<commit_message>
Cambio en las rutas de la generación de archivos
</commit_message>
<xml_diff>
--- a/sujetos.xlsx
+++ b/sujetos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,19 +496,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>37291</v>
+        <v>36651</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BACHILLERATO</t>
+          <t>MAESTRÍA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>INBI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -518,22 +518,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>samuel.ceballos4453@alumnos.udg.mx</t>
+          <t>marco@gmail.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3311111111</t>
+          <t>3322222222</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -543,19 +543,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>38842</v>
+        <v>36651</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BACHILLERATO</t>
+          <t>MAESTRÍA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>INCO</t>
+          <t>INBI</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -565,24 +565,165 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>franco.silva4477@alumnos.udg.mx</t>
+          <t>marco@gmail.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>3355669988</t>
+          <t>3322222222</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K3" t="inlineStr">
+        <is>
+          <t>Charm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>36651</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MAESTRÍA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INBI</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>marco@gmail.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>3322222222</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Charm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>36651</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MAESTRÍA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INBI</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>marco@gmail.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>3322222222</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Charm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>36651</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MAESTRÍA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>INBI</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>marco@gmail.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>3322222222</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Charm1</t>
         </is>

</xml_diff>